<commit_message>
optimize index case group
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/index/index_cases1_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/index/index_cases1_btree.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$257</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -5046,8 +5046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I230" sqref="I230"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C261" sqref="C261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5110,7 +5110,7 @@
         <v>819</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>327</v>
@@ -5145,7 +5145,7 @@
         <v>820</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>817</v>
@@ -5180,7 +5180,7 @@
         <v>821</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>818</v>
@@ -5215,7 +5215,7 @@
         <v>822</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>328</v>
@@ -5250,7 +5250,7 @@
         <v>823</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>329</v>
@@ -5285,7 +5285,7 @@
         <v>824</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>330</v>
@@ -5320,7 +5320,7 @@
         <v>825</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>331</v>
@@ -5355,7 +5355,7 @@
         <v>826</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>33</v>
@@ -5390,7 +5390,7 @@
         <v>827</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>36</v>
@@ -5425,7 +5425,7 @@
         <v>828</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>40</v>
@@ -5460,7 +5460,7 @@
         <v>829</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>44</v>
@@ -5495,7 +5495,7 @@
         <v>830</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>48</v>
@@ -5530,7 +5530,7 @@
         <v>831</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>52</v>
@@ -5565,7 +5565,7 @@
         <v>832</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>56</v>
@@ -5600,7 +5600,7 @@
         <v>833</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>74</v>
@@ -5635,7 +5635,7 @@
         <v>834</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>75</v>
@@ -5670,7 +5670,7 @@
         <v>835</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>76</v>
@@ -5705,7 +5705,7 @@
         <v>836</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>77</v>
@@ -5740,7 +5740,7 @@
         <v>837</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>78</v>
@@ -5775,7 +5775,7 @@
         <v>838</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>79</v>
@@ -5845,7 +5845,7 @@
         <v>840</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>332</v>
@@ -5880,7 +5880,7 @@
         <v>841</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>333</v>
@@ -5915,7 +5915,7 @@
         <v>842</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>537</v>
@@ -5950,7 +5950,7 @@
         <v>843</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>538</v>
@@ -5985,7 +5985,7 @@
         <v>844</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>539</v>
@@ -6020,7 +6020,7 @@
         <v>845</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>540</v>
@@ -6090,7 +6090,7 @@
         <v>847</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>136</v>
@@ -6125,7 +6125,7 @@
         <v>848</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>110</v>
@@ -6160,7 +6160,7 @@
         <v>849</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>111</v>
@@ -6195,7 +6195,7 @@
         <v>850</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>112</v>
@@ -6230,7 +6230,7 @@
         <v>851</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>113</v>
@@ -6265,7 +6265,7 @@
         <v>852</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>114</v>
@@ -6300,7 +6300,7 @@
         <v>853</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>115</v>
@@ -6335,7 +6335,7 @@
         <v>854</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>137</v>
@@ -6370,7 +6370,7 @@
         <v>855</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>138</v>
@@ -6405,7 +6405,7 @@
         <v>856</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>139</v>
@@ -6440,7 +6440,7 @@
         <v>857</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>140</v>
@@ -6475,7 +6475,7 @@
         <v>858</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>141</v>
@@ -6510,7 +6510,7 @@
         <v>859</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>142</v>
@@ -6545,7 +6545,7 @@
         <v>860</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>143</v>
@@ -6615,7 +6615,7 @@
         <v>919</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>165</v>
@@ -6685,7 +6685,7 @@
         <v>921</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>167</v>
@@ -6720,7 +6720,7 @@
         <v>922</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>168</v>
@@ -6790,7 +6790,7 @@
         <v>924</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>170</v>
@@ -6825,7 +6825,7 @@
         <v>925</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>171</v>
@@ -6860,7 +6860,7 @@
         <v>926</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>172</v>
@@ -7032,7 +7032,7 @@
         <v>931</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>198</v>
@@ -7067,7 +7067,7 @@
         <v>932</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>203</v>
@@ -7102,7 +7102,7 @@
         <v>933</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>210</v>
@@ -7137,7 +7137,7 @@
         <v>934</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>211</v>
@@ -7172,7 +7172,7 @@
         <v>935</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>212</v>
@@ -7207,7 +7207,7 @@
         <v>936</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>213</v>
@@ -7242,7 +7242,7 @@
         <v>937</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>221</v>
@@ -7277,7 +7277,7 @@
         <v>938</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>222</v>
@@ -7312,7 +7312,7 @@
         <v>939</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>227</v>
@@ -7347,7 +7347,7 @@
         <v>940</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>230</v>
@@ -7382,7 +7382,7 @@
         <v>941</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>232</v>
@@ -7417,7 +7417,7 @@
         <v>942</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>236</v>
@@ -7452,7 +7452,7 @@
         <v>943</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>238</v>
@@ -7487,7 +7487,7 @@
         <v>944</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>241</v>
@@ -7522,7 +7522,7 @@
         <v>945</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>244</v>
@@ -7557,7 +7557,7 @@
         <v>946</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>247</v>
@@ -7592,7 +7592,7 @@
         <v>947</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>248</v>
@@ -7627,7 +7627,7 @@
         <v>948</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>253</v>
@@ -7662,7 +7662,7 @@
         <v>949</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>257</v>
@@ -7697,7 +7697,7 @@
         <v>950</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>260</v>
@@ -7732,7 +7732,7 @@
         <v>951</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>264</v>
@@ -7767,7 +7767,7 @@
         <v>952</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>274</v>
@@ -7802,7 +7802,7 @@
         <v>953</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>277</v>
@@ -7837,7 +7837,7 @@
         <v>954</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>276</v>
@@ -7872,7 +7872,7 @@
         <v>955</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>279</v>
@@ -7907,7 +7907,7 @@
         <v>956</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>281</v>
@@ -7942,7 +7942,7 @@
         <v>957</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>283</v>
@@ -7977,7 +7977,7 @@
         <v>958</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>284</v>
@@ -8012,7 +8012,7 @@
         <v>959</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>285</v>
@@ -8047,7 +8047,7 @@
         <v>960</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>290</v>
@@ -8082,7 +8082,7 @@
         <v>961</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>295</v>
@@ -8117,7 +8117,7 @@
         <v>962</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>296</v>
@@ -8152,7 +8152,7 @@
         <v>963</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>297</v>
@@ -8187,7 +8187,7 @@
         <v>964</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>302</v>
@@ -8222,7 +8222,7 @@
         <v>965</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>303</v>
@@ -8257,7 +8257,7 @@
         <v>966</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>304</v>
@@ -8292,7 +8292,7 @@
         <v>967</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>318</v>
@@ -8327,7 +8327,7 @@
         <v>968</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>311</v>
@@ -8362,7 +8362,7 @@
         <v>969</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>312</v>
@@ -8397,7 +8397,7 @@
         <v>970</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>323</v>
@@ -8432,7 +8432,7 @@
         <v>971</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>324</v>
@@ -8467,7 +8467,7 @@
         <v>861</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>339</v>
@@ -8537,7 +8537,7 @@
         <v>863</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>345</v>
@@ -8572,7 +8572,7 @@
         <v>864</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>351</v>
@@ -8607,7 +8607,7 @@
         <v>865</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>346</v>
@@ -8642,7 +8642,7 @@
         <v>866</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>347</v>
@@ -8677,7 +8677,7 @@
         <v>867</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>358</v>
@@ -8712,7 +8712,7 @@
         <v>868</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>361</v>
@@ -8747,7 +8747,7 @@
         <v>869</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>362</v>
@@ -8782,7 +8782,7 @@
         <v>870</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>363</v>
@@ -8817,7 +8817,7 @@
         <v>871</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>364</v>
@@ -8852,7 +8852,7 @@
         <v>872</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>365</v>
@@ -8887,7 +8887,7 @@
         <v>873</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>374</v>
@@ -8922,7 +8922,7 @@
         <v>874</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>372</v>
@@ -8957,7 +8957,7 @@
         <v>875</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>373</v>
@@ -8992,7 +8992,7 @@
         <v>876</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>382</v>
@@ -9027,7 +9027,7 @@
         <v>877</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>383</v>
@@ -9196,11 +9196,11 @@
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="5" t="s">
         <v>882</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>399</v>
@@ -9231,11 +9231,11 @@
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="5" t="s">
         <v>883</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>400</v>
@@ -11132,7 +11132,7 @@
         <v>972</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>526</v>
@@ -11167,7 +11167,7 @@
         <v>973</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>527</v>
@@ -11202,7 +11202,7 @@
         <v>974</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>528</v>
@@ -11237,7 +11237,7 @@
         <v>975</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>529</v>
@@ -11272,7 +11272,7 @@
         <v>976</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>555</v>
@@ -11304,7 +11304,7 @@
         <v>1001</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>568</v>
@@ -11336,7 +11336,7 @@
         <v>1002</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>569</v>
@@ -11368,7 +11368,7 @@
         <v>1003</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>558</v>
@@ -11403,7 +11403,7 @@
         <v>1004</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>559</v>
@@ -11438,7 +11438,7 @@
         <v>1005</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>570</v>
@@ -11470,7 +11470,7 @@
         <v>1006</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>571</v>
@@ -11502,7 +11502,7 @@
         <v>1007</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>572</v>
@@ -11534,7 +11534,7 @@
         <v>1008</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>573</v>
@@ -11566,7 +11566,7 @@
         <v>1009</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>585</v>
@@ -11601,7 +11601,7 @@
         <v>1010</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>586</v>
@@ -11636,7 +11636,7 @@
         <v>1011</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>587</v>
@@ -11671,7 +11671,7 @@
         <v>1012</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>588</v>
@@ -11706,7 +11706,7 @@
         <v>1013</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>589</v>
@@ -11741,7 +11741,7 @@
         <v>1014</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>590</v>
@@ -11776,7 +11776,7 @@
         <v>1015</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>591</v>
@@ -11811,7 +11811,7 @@
         <v>1016</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>592</v>
@@ -11846,7 +11846,7 @@
         <v>1017</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>593</v>
@@ -11881,7 +11881,7 @@
         <v>1018</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>594</v>
@@ -11916,7 +11916,7 @@
         <v>1019</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>595</v>
@@ -11986,7 +11986,7 @@
         <v>1021</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>597</v>
@@ -12021,7 +12021,7 @@
         <v>1022</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>598</v>
@@ -12056,7 +12056,7 @@
         <v>1023</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>599</v>
@@ -12091,7 +12091,7 @@
         <v>1024</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>600</v>
@@ -12126,7 +12126,7 @@
         <v>1025</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>601</v>
@@ -12161,7 +12161,7 @@
         <v>1026</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>602</v>
@@ -12196,7 +12196,7 @@
         <v>1027</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>603</v>
@@ -12231,7 +12231,7 @@
         <v>1028</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>604</v>
@@ -12301,7 +12301,7 @@
         <v>1030</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>606</v>
@@ -12371,7 +12371,7 @@
         <v>1032</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>608</v>
@@ -12406,7 +12406,7 @@
         <v>1033</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>609</v>
@@ -12581,7 +12581,7 @@
         <v>1038</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>703</v>
@@ -12616,7 +12616,7 @@
         <v>1039</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>704</v>
@@ -12718,7 +12718,7 @@
         <v>1042</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>684</v>
@@ -12750,7 +12750,7 @@
         <v>1043</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>685</v>
@@ -12782,7 +12782,7 @@
         <v>1044</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>686</v>
@@ -12810,7 +12810,7 @@
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="4" t="s">
         <v>1045</v>
       </c>
       <c r="B228" s="3" t="s">
@@ -12919,7 +12919,7 @@
         <v>1048</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>716</v>
@@ -12954,7 +12954,7 @@
         <v>1049</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>717</v>
@@ -12989,7 +12989,7 @@
         <v>1050</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>718</v>
@@ -13024,7 +13024,7 @@
         <v>1051</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>719</v>
@@ -13059,7 +13059,7 @@
         <v>1052</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>720</v>
@@ -13094,7 +13094,7 @@
         <v>1053</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>721</v>
@@ -13129,7 +13129,7 @@
         <v>1054</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>722</v>
@@ -13164,7 +13164,7 @@
         <v>1055</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>723</v>
@@ -13199,7 +13199,7 @@
         <v>1056</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>742</v>
@@ -13234,7 +13234,7 @@
         <v>1057</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>746</v>
@@ -13269,7 +13269,7 @@
         <v>1058</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>757</v>
@@ -13304,7 +13304,7 @@
         <v>1059</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>758</v>
@@ -13339,7 +13339,7 @@
         <v>1060</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>763</v>
@@ -13374,7 +13374,7 @@
         <v>1061</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>765</v>
@@ -13409,7 +13409,7 @@
         <v>1062</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>766</v>
@@ -13444,7 +13444,7 @@
         <v>1063</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>767</v>
@@ -13479,7 +13479,7 @@
         <v>1064</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>785</v>
@@ -13514,7 +13514,7 @@
         <v>1065</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>786</v>
@@ -13549,7 +13549,7 @@
         <v>1066</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>788</v>
@@ -13584,7 +13584,7 @@
         <v>1067</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>791</v>
@@ -13619,7 +13619,7 @@
         <v>1068</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>793</v>
@@ -13654,7 +13654,7 @@
         <v>1069</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>794</v>
@@ -13689,7 +13689,7 @@
         <v>1070</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>795</v>
@@ -13724,7 +13724,7 @@
         <v>1071</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>796</v>
@@ -13759,7 +13759,7 @@
         <v>1072</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>806</v>
@@ -13860,7 +13860,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L2"/>
+  <autoFilter ref="A1:L257"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">

</xml_diff>